<commit_message>
update New Data Process code
</commit_message>
<xml_diff>
--- a/Code/Problem2/Data/Data.xlsx
+++ b/Code/Problem2/Data/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\丁智\OneDrive - zju.edu.cn\浙江大学\研究资料\毕业设计\Optimization-Plan-for-Emergency-Evacuation-of-Personnel-Based-on-Genetic-Algorithm\Code\Problem2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87B7C44-F2E1-4CEB-9511-F7D81D71ADF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B97059-E4C9-48D4-96B6-05A0ABAB1F1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="31196" windowHeight="17038" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -428,23 +428,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="25.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="8.88671875" style="1"/>
-    <col min="9" max="9" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="25.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="8.875" style="1"/>
+    <col min="9" max="9" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="52" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="11" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
@@ -455,7 +455,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -465,7 +465,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -479,134 +479,148 @@
         <v>650</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>400</v>
+      </c>
+      <c r="C4" s="1">
+        <v>400</v>
+      </c>
+      <c r="D4" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>760</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>880</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D6" s="1">
         <v>670</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="1">
         <v>210</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <v>240</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D7" s="1">
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="1">
         <v>100</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <v>200</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D8" s="1">
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="1">
         <v>750</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C10" s="1">
         <v>950</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D10" s="1">
         <v>650</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11" s="1">
         <v>210</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>250</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <v>230</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>150</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <v>200</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D12" s="1">
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B5:D5"/>
     <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B44:D44"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>